<commit_message>
Escreve em ficheiros excel, guarda nome da classe, package e método, a o
</commit_message>
<xml_diff>
--- a/Excel Files/Teste2.xlsx
+++ b/Excel Files/Teste2.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7CC0C4B1-B5A5-4673-8F70-5374CFAE0CA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Code Smells" r:id="rId3" sheetId="1"/>
+    <sheet name="Code Smells" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="100">
   <si>
     <t>MethodID</t>
   </si>
@@ -56,7 +60,7 @@
     <t>ExcelExporting.java</t>
   </si>
   <si>
-    <t>métodos</t>
+    <t>ExcelExporting</t>
   </si>
   <si>
     <t>4</t>
@@ -86,6 +90,9 @@
     <t>RandomizedQueue.java</t>
   </si>
   <si>
+    <t>enqueue</t>
+  </si>
+  <si>
     <t>12</t>
   </si>
   <si>
@@ -101,60 +108,102 @@
     <t>11</t>
   </si>
   <si>
+    <t>dequeue</t>
+  </si>
+  <si>
     <t>19</t>
   </si>
   <si>
+    <t>sample</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
     <t>13</t>
   </si>
   <si>
+    <t>iterator</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
+    <t>main</t>
+  </si>
+  <si>
     <t>26</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
+    <t>randomQueueIterator</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
+    <t>hasNext</t>
+  </si>
+  <si>
     <t>17</t>
   </si>
   <si>
+    <t>next</t>
+  </si>
+  <si>
     <t>9</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
+    <t>remove</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
     <t>SmellyClass.java</t>
   </si>
   <si>
-    <t>346</t>
-  </si>
-  <si>
-    <t>101</t>
+    <t>SmellyClass</t>
+  </si>
+  <si>
+    <t>341</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>exportToExcel</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
+    <t>NOM</t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>WMC</t>
+  </si>
+  <si>
     <t>23</t>
   </si>
   <si>
+    <t>LOC_Method</t>
+  </si>
+  <si>
     <t>25</t>
   </si>
   <si>
@@ -164,62 +213,118 @@
     <t>27</t>
   </si>
   <si>
+    <t>CYCLO_Method</t>
+  </si>
+  <si>
     <t>28</t>
   </si>
   <si>
+    <t>isGodClass</t>
+  </si>
+  <si>
     <t>95</t>
   </si>
   <si>
     <t>40</t>
   </si>
   <si>
+    <t>setClassAndPackageNames</t>
+  </si>
+  <si>
     <t>30</t>
   </si>
   <si>
+    <t>isLongMethod</t>
+  </si>
+  <si>
     <t>50</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
+    <t>LOC_Class</t>
+  </si>
+  <si>
     <t>32</t>
   </si>
   <si>
+    <t>methodName</t>
+  </si>
+  <si>
     <t>33</t>
   </si>
   <si>
+    <t>getMethod</t>
+  </si>
+  <si>
     <t>34</t>
   </si>
   <si>
+    <t>getLinesOfCode</t>
+  </si>
+  <si>
     <t>35</t>
   </si>
   <si>
+    <t>getLinesPerMethod</t>
+  </si>
+  <si>
     <t>36</t>
   </si>
   <si>
+    <t>getAreLongMethods</t>
+  </si>
+  <si>
     <t>37</t>
   </si>
   <si>
+    <t>getCyclosPerMethod</t>
+  </si>
+  <si>
     <t>38</t>
   </si>
   <si>
+    <t>getisGodClass</t>
+  </si>
+  <si>
     <t>39</t>
   </si>
   <si>
+    <t>getWmcCount</t>
+  </si>
+  <si>
+    <t>chooseName</t>
+  </si>
+  <si>
+    <t>getMethodNames</t>
+  </si>
+  <si>
     <t>Main.java</t>
   </si>
   <si>
+    <t>restartReading</t>
+  </si>
+  <si>
     <t>56</t>
+  </si>
+  <si>
+    <t>RandomizedQueue</t>
+  </si>
+  <si>
+    <t>isEmpty</t>
+  </si>
+  <si>
+    <t>size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -231,7 +336,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -249,18 +354,331 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:K20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="43.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -295,7 +713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -330,7 +748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -341,22 +759,22 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
@@ -365,9 +783,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -376,22 +794,22 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
         <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -400,9 +818,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -411,22 +829,22 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
@@ -435,9 +853,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -446,22 +864,22 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
         <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
         <v>11</v>
@@ -470,9 +888,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -481,22 +899,22 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
         <v>18</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
@@ -505,9 +923,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -516,22 +934,22 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
         <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J8" t="s">
         <v>20</v>
@@ -540,9 +958,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -551,22 +969,22 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
         <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
@@ -575,9 +993,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -586,33 +1004,33 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -621,22 +1039,22 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
         <v>18</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J11" t="s">
         <v>11</v>
@@ -645,27 +1063,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H12" t="s">
         <v>18</v>
@@ -680,7 +1098,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -691,7 +1109,7 @@
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -706,42 +1124,42 @@
         <v>18</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="J13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H14" t="s">
         <v>18</v>
       </c>
       <c r="I14" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J14" t="s">
         <v>20</v>
@@ -750,33 +1168,33 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s">
         <v>18</v>
       </c>
       <c r="I15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J15" t="s">
         <v>11</v>
@@ -785,33 +1203,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" t="s">
-        <v>35</v>
       </c>
       <c r="J16" t="s">
         <v>20</v>
@@ -820,33 +1238,33 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H17" t="s">
         <v>18</v>
       </c>
       <c r="I17" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="J17" t="s">
         <v>11</v>
@@ -855,7 +1273,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -863,19 +1281,19 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H18" t="s">
         <v>18</v>
@@ -890,103 +1308,103 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H19" t="s">
         <v>18</v>
       </c>
       <c r="I19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J19" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G20" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H20" t="s">
         <v>18</v>
       </c>
       <c r="I20" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="J20" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="K20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G21" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H21" t="s">
         <v>18</v>
       </c>
       <c r="I21" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J21" t="s">
         <v>20</v>
@@ -995,79 +1413,79 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G22" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H22" t="s">
         <v>18</v>
       </c>
       <c r="I22" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="J22" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G23" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H23" t="s">
         <v>18</v>
       </c>
       <c r="I23" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="J23" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="K23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
@@ -1076,7 +1494,7 @@
         <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
@@ -1100,68 +1518,68 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" t="s">
-        <v>43</v>
-      </c>
       <c r="H25" t="s">
         <v>18</v>
       </c>
       <c r="I25" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="J25" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="K25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
       <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" t="s">
         <v>41</v>
-      </c>
-      <c r="D26" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" t="s">
-        <v>43</v>
-      </c>
-      <c r="H26" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" t="s">
-        <v>35</v>
       </c>
       <c r="J26" t="s">
         <v>11</v>
@@ -1170,33 +1588,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H27" t="s">
         <v>18</v>
       </c>
       <c r="I27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J27" t="s">
         <v>11</v>
@@ -1205,33 +1623,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G28" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H28" t="s">
         <v>18</v>
       </c>
       <c r="I28" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J28" t="s">
         <v>11</v>
@@ -1240,33 +1658,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F29" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G29" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H29" t="s">
         <v>18</v>
       </c>
       <c r="I29" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J29" t="s">
         <v>11</v>
@@ -1275,33 +1693,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G30" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H30" t="s">
         <v>18</v>
       </c>
       <c r="I30" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J30" t="s">
         <v>11</v>
@@ -1310,33 +1728,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G31" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H31" t="s">
         <v>18</v>
       </c>
       <c r="I31" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J31" t="s">
         <v>11</v>
@@ -1345,33 +1763,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G32" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H32" t="s">
         <v>18</v>
       </c>
       <c r="I32" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J32" t="s">
         <v>11</v>
@@ -1380,33 +1798,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G33" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H33" t="s">
         <v>18</v>
       </c>
       <c r="I33" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J33" t="s">
         <v>11</v>
@@ -1415,27 +1833,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F34" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G34" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H34" t="s">
         <v>18</v>
@@ -1450,7 +1868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -1461,7 +1879,7 @@
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -1485,27 +1903,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" t="s">
         <v>52</v>
       </c>
-      <c r="B36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" t="s">
-        <v>42</v>
-      </c>
       <c r="G36" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H36" t="s">
         <v>18</v>
@@ -1520,79 +1938,79 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="E37" t="s">
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="G37" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H37" t="s">
         <v>18</v>
       </c>
       <c r="I37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" t="s">
         <v>36</v>
-      </c>
-      <c r="J37" t="s">
-        <v>32</v>
       </c>
       <c r="K37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="E38" t="s">
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="G38" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H38" t="s">
         <v>18</v>
       </c>
       <c r="I38" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="J38" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
         <v>12</v>
@@ -1601,16 +2019,16 @@
         <v>23</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G39" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H39" t="s">
         <v>18</v>
@@ -1625,7 +2043,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -1636,22 +2054,22 @@
         <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G40" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H40" t="s">
         <v>18</v>
       </c>
       <c r="I40" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J40" t="s">
         <v>11</v>
@@ -1660,9 +2078,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
         <v>12</v>
@@ -1671,22 +2089,22 @@
         <v>23</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="E41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G41" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H41" t="s">
         <v>18</v>
       </c>
       <c r="I41" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J41" t="s">
         <v>11</v>
@@ -1696,6 +2114,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>